<commit_message>
Tarea realizada plus cambios en metodos
</commit_message>
<xml_diff>
--- a/AutomationCooltestersJuly/src/test/resources/testData/excel/Orange_test_POM.xlsx
+++ b/AutomationCooltestersJuly/src/test/resources/testData/excel/Orange_test_POM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trulu pc\git\AutomationCooltesterJuly\AutomationCooltestersJuly\src\test\resources\testData\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A052EBBE-88DC-4674-9068-A2184C5D1B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FD581D-C74A-4B50-B7BE-1ABFA2263E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Username</t>
   </si>
@@ -66,7 +66,37 @@
     <t>Nina Patel</t>
   </si>
   <si>
-    <t>Trulu.test</t>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>userToDelete</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ESS</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>TruluTest.test</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t>Trulu.Disabled2.11</t>
+  </si>
+  <si>
+    <t>Trulu.Disabled2.2</t>
   </si>
 </sst>
 </file>
@@ -90,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -173,11 +203,115 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -185,9 +319,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,34 +611,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="I1" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -505,17 +653,26 @@
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="14" t="s">
         <v>11</v>
       </c>
+      <c r="G2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -525,14 +682,67 @@
       <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>13</v>
+      <c r="F3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -541,6 +751,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EA119EE9BB2D674889D7A1A8D57BB3DB" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="53489c467ea4bbbf05319f6c3a3f022f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="75acaddb-6f44-4feb-ad56-7fa24623e226" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3fbb944b84beadbbfffc42b944bbfd13" ns2:_="">
     <xsd:import namespace="75acaddb-6f44-4feb-ad56-7fa24623e226"/>
@@ -702,15 +921,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -718,6 +928,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F300B6A8-6660-4860-84F1-D7B0F0D085E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E9A6DBE-7B07-4173-A8E8-174CE99B65EB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -735,14 +953,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F300B6A8-6660-4860-84F1-D7B0F0D085E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6492C325-9E95-4CDB-893C-39C8900DD5A0}">
   <ds:schemaRefs>

</xml_diff>